<commit_message>
Poprawa polskich znaków w tabelkach
</commit_message>
<xml_diff>
--- a/Generator/Generator.xlsx
+++ b/Generator/Generator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateusz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\BD2_repo\BDProject\Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -669,12 +669,6 @@
     <t>KOWALSKI</t>
   </si>
   <si>
-    <t>WINIEWSKA</t>
-  </si>
-  <si>
-    <t>WINIEWSKI</t>
-  </si>
-  <si>
     <t>WÓJCIK</t>
   </si>
   <si>
@@ -693,12 +687,6 @@
     <t>LEWANDOWSKI</t>
   </si>
   <si>
-    <t>DĽBROWSKA</t>
-  </si>
-  <si>
-    <t>DĽBROWSKI</t>
-  </si>
-  <si>
     <t>ZIELIŃSKA</t>
   </si>
   <si>
@@ -711,9 +699,6 @@
     <t>SZYMAŃSKI</t>
   </si>
   <si>
-    <t>WONIAK</t>
-  </si>
-  <si>
     <t>KOZŁOWSKA</t>
   </si>
   <si>
@@ -762,9 +747,6 @@
     <t>PAWŁOWSKA</t>
   </si>
   <si>
-    <t>ZAJĽC</t>
-  </si>
-  <si>
     <t>MICHALSKA</t>
   </si>
   <si>
@@ -1129,6 +1111,24 @@
   </si>
   <si>
     <t>Aquaworld</t>
+  </si>
+  <si>
+    <t>DĄBROWSKI</t>
+  </si>
+  <si>
+    <t>WIŚNIEWSKI</t>
+  </si>
+  <si>
+    <t>WOŹNIAK</t>
+  </si>
+  <si>
+    <t>ZAJĄC</t>
+  </si>
+  <si>
+    <t>WIŚNIEWSKA</t>
+  </si>
+  <si>
+    <t>DĄBROWSKA</t>
   </si>
 </sst>
 </file>
@@ -2185,22 +2185,22 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>124</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>128</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>130</v>
       </c>
@@ -2245,17 +2245,17 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>135</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>140</v>
       </c>
@@ -2300,12 +2300,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>145</v>
       </c>
@@ -2330,12 +2330,12 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>151</v>
       </c>
@@ -2365,12 +2365,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>158</v>
       </c>
@@ -2380,17 +2380,17 @@
         <v>159</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>162</v>
       </c>
@@ -2405,12 +2405,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>166</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>169</v>
       </c>
@@ -2470,12 +2470,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>179</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>185</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>187</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>192</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>194</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>198</v>
       </c>
@@ -2590,7 +2590,7 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2612,345 +2612,345 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>212</v>
+        <v>351</v>
       </c>
       <c r="B8" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B9" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B10" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>217</v>
+        <v>353</v>
       </c>
       <c r="B11" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B12" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B13" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B15" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B16" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B17" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B18" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B19" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B20" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>234</v>
+        <v>354</v>
       </c>
       <c r="B21" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B22" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B23" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B24" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B25" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B26" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B27" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B28" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B29" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B30" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B31" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B32" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B33" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B34" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B35" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B36" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B37" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B38" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B39" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B40" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B41" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B42" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -2963,7 +2963,7 @@
   <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2983,202 +2983,202 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>217</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>234</v>
+        <v>354</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -3201,277 +3201,277 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3494,177 +3494,177 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodanie zawodów do generatora (męskie i żeńskie ;) )
</commit_message>
<xml_diff>
--- a/Generator/Generator.xlsx
+++ b/Generator/Generator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Imiona męskie" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="Hasła" sheetId="9" r:id="rId8"/>
     <sheet name="Loginy" sheetId="10" r:id="rId9"/>
     <sheet name="Usługi" sheetId="11" r:id="rId10"/>
+    <sheet name="Stanowiska męskie" sheetId="12" r:id="rId11"/>
+    <sheet name="Stanowiska żeńskie" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_603_116k_ipb_found" localSheetId="8">Loginy!$A$1:$A$1104</definedName>
@@ -79,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3768" uniqueCount="3545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3782" uniqueCount="3558">
   <si>
     <t>Antoni</t>
   </si>
@@ -10714,6 +10716,45 @@
   </si>
   <si>
     <t>squash</t>
+  </si>
+  <si>
+    <t>ekspert ds. marketingu</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>kasjer</t>
+  </si>
+  <si>
+    <t>kierownik</t>
+  </si>
+  <si>
+    <t>konserwator</t>
+  </si>
+  <si>
+    <t>ratownik</t>
+  </si>
+  <si>
+    <t>sprzątaczka</t>
+  </si>
+  <si>
+    <t>sprzątacz</t>
+  </si>
+  <si>
+    <t>ekspertka ds. marketingu</t>
+  </si>
+  <si>
+    <t>kasjerka</t>
+  </si>
+  <si>
+    <t>kierowniczka</t>
+  </si>
+  <si>
+    <t>konserwatorka</t>
+  </si>
+  <si>
+    <t>ratowniczka</t>
   </si>
 </sst>
 </file>
@@ -11729,6 +11770,112 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3545</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3546</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3547</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3548</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3549</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3550</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3552</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3553</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3546</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3556</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3557</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3551</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A100"/>
@@ -19221,7 +19368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>

</xml_diff>